<commit_message>
Update grades_tally and L16
</commit_message>
<xml_diff>
--- a/data/grades_tally.xlsx
+++ b/data/grades_tally.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Documents\GitHub\M221R\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CBA5973D-5AAF-49DB-B1C1-B174FDCF1771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E829AADA-EE2D-4675-91D7-A4AB718272F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-8205" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="grades" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>A</t>
   </si>
@@ -64,13 +64,10 @@
     <t xml:space="preserve">Tally of final grades of </t>
   </si>
   <si>
-    <t xml:space="preserve">Summarized from </t>
-  </si>
-  <si>
     <t>course at BYU-Idaho.</t>
   </si>
   <si>
-    <t>grades_gender.xlsx</t>
+    <t>Summarized from grades_gender.xlsx</t>
   </si>
 </sst>
 </file>
@@ -913,9 +910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -960,7 +955,7 @@
         <v>61</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -971,7 +966,7 @@
         <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -980,9 +975,6 @@
       </c>
       <c r="B6">
         <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>